<commit_message>
Added reset button for LHCbit
</commit_message>
<xml_diff>
--- a/LHCbit/altium/LHCbit/BOM/BOM_JLCPCB-LHCbit.xlsx
+++ b/LHCbit/altium/LHCbit/BOM/BOM_JLCPCB-LHCbit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leand\Documents\Altium\Projetos\LHC\LHCbit\LHCbit\LHCbit\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leand\Documents\Altium\Projetos\LHC\LHCbit\LHCbit\altium\LHCbit\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4D15355-1BE4-420E-B6B7-A634F6002062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F0F46F8-5FA2-42CE-900C-6E6D5590ACE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="38700" windowHeight="15285" xr2:uid="{443E0804-E6AE-44AE-8E2D-54130479CC37}"/>
+    <workbookView xWindow="1650" yWindow="1905" windowWidth="21600" windowHeight="11295" xr2:uid="{5C9E7839-CE02-4E8B-A94C-1F460B2A56AF}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_JLCPCB-LHCbit" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="90">
   <si>
     <t>Designator</t>
   </si>
@@ -68,6 +68,21 @@
     <t/>
   </si>
   <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>WS-TASV 3.5x2.9mm Tact Switch, J-Bend SMD version</t>
+  </si>
+  <si>
+    <t>Wurth Elektronik</t>
+  </si>
+  <si>
+    <t>434153017835</t>
+  </si>
+  <si>
+    <t>Switches</t>
+  </si>
+  <si>
     <t>LED1</t>
   </si>
   <si>
@@ -146,13 +161,7 @@
     <t>WS-TASV 6x6mm Tact Switch, SMD version</t>
   </si>
   <si>
-    <t>Wurth Elektronik</t>
-  </si>
-  <si>
     <t>DTSM-6</t>
-  </si>
-  <si>
-    <t>Switches</t>
   </si>
   <si>
     <t>U1</t>
@@ -695,8 +704,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C5B777F-0AFD-4E20-9E30-04D30F2E570E}">
-  <dimension ref="A1:G23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B74F786-33EE-466D-8130-A17DBD015E86}">
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -757,27 +766,25 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="B4" s="1"/>
       <c r="C4" s="1">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -797,294 +804,294 @@
         <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C6" s="1">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="F8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C11" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="G11" s="2" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>49</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="C15" s="1">
-        <v>2</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>57</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="1"/>
       <c r="C16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C17" s="1">
-        <v>6</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>64</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1095,37 +1102,41 @@
         <v>66</v>
       </c>
       <c r="C18" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G18" s="1"/>
+      <c r="G18" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="1"/>
       <c r="C19" s="1">
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="1"/>
       <c r="F19" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -1136,21 +1147,19 @@
         <v>1</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="2" t="s">
         <v>73</v>
       </c>
+      <c r="E20" s="1"/>
       <c r="F20" s="2" t="s">
         <v>74</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>75</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1">
@@ -1160,12 +1169,14 @@
         <v>8</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -1176,43 +1187,62 @@
         <v>1</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="1">
+      <c r="F23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="1">
         <v>3</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>50</v>
+      <c r="D24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Improved silkscreen of LHCbit
</commit_message>
<xml_diff>
--- a/LHCbit/altium/LHCbit/BOM/BOM_JLCPCB-LHCbit.xlsx
+++ b/LHCbit/altium/LHCbit/BOM/BOM_JLCPCB-LHCbit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leand\Documents\Altium\Projetos\LHC\LHCbit\LHCbit\altium\LHCbit\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F0F46F8-5FA2-42CE-900C-6E6D5590ACE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1638AD8-3C83-4449-8B2E-902951EE7A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1650" yWindow="1905" windowWidth="21600" windowHeight="11295" xr2:uid="{5C9E7839-CE02-4E8B-A94C-1F460B2A56AF}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{748367B0-0E6D-463C-99F8-DEB9387A8DB7}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_JLCPCB-LHCbit" sheetId="1" r:id="rId1"/>
@@ -704,22 +704,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B74F786-33EE-466D-8130-A17DBD015E86}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDD2999A-EA8F-46C0-884E-9BEB0CDBEB1F}">
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" customWidth="1"/>
+    <col min="3" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -742,7 +742,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -757,7 +757,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -778,7 +778,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -799,7 +799,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -822,7 +822,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -845,7 +845,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -868,7 +868,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
@@ -891,7 +891,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>33</v>
       </c>
@@ -914,7 +914,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
@@ -937,7 +937,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>38</v>
       </c>
@@ -960,7 +960,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>41</v>
       </c>
@@ -981,7 +981,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>46</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>50</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>54</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>58</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>62</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>65</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>68</v>
       </c>
@@ -1138,7 +1138,7 @@
       </c>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>72</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>75</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>79</v>
       </c>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>82</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>86</v>
       </c>

</xml_diff>

<commit_message>
Changed button s2 to IO0 and added header for uart
</commit_message>
<xml_diff>
--- a/LHCbit/altium/LHCbit/BOM/BOM_JLCPCB-LHCbit.xlsx
+++ b/LHCbit/altium/LHCbit/BOM/BOM_JLCPCB-LHCbit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leand\Documents\Altium\Projetos\LHC\LHCbit\LHCbit\altium\LHCbit\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1638AD8-3C83-4449-8B2E-902951EE7A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7698AB3F-DDF4-45F2-88D4-09AE247BDF9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{748367B0-0E6D-463C-99F8-DEB9387A8DB7}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{003AB811-9858-45E1-8E95-0D66E6A8E10F}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_JLCPCB-LHCbit" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="94">
   <si>
     <t>Designator</t>
   </si>
@@ -68,13 +68,25 @@
     <t/>
   </si>
   <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>WR-PHD 2.00 mm THT Pin Header, 4p</t>
+  </si>
+  <si>
+    <t>Wurth Elektronik</t>
+  </si>
+  <si>
+    <t>62000411121</t>
+  </si>
+  <si>
     <t>S3</t>
   </si>
   <si>
     <t>WS-TASV 3.5x2.9mm Tact Switch, J-Bend SMD version</t>
-  </si>
-  <si>
-    <t>Wurth Elektronik</t>
   </si>
   <si>
     <t>434153017835</t>
@@ -704,8 +716,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDD2999A-EA8F-46C0-884E-9BEB0CDBEB1F}">
-  <dimension ref="A1:G24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17900F69-286B-4421-9E34-75C9DEA2AEAF}">
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -761,22 +773,22 @@
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -787,10 +799,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>16</v>
@@ -803,34 +815,32 @@
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="1">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="C6" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -842,18 +852,18 @@
         <v>25</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -865,7 +875,7 @@
         <v>29</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -876,132 +886,132 @@
         <v>31</v>
       </c>
       <c r="C8" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C11" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>44</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1018,13 +1028,13 @@
         <v>8</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1041,13 +1051,13 @@
         <v>8</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1058,124 +1068,126 @@
         <v>59</v>
       </c>
       <c r="C16" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="C17" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>64</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" s="2" t="s">
         <v>66</v>
       </c>
+      <c r="B18" s="1"/>
       <c r="C18" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C19" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G19" s="1"/>
+      <c r="G19" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="1"/>
+      <c r="B20" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="C20" s="1">
         <v>1</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="F20" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1">
         <v>1</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>76</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="E21" s="1"/>
       <c r="F21" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1195,18 +1207,20 @@
       <c r="F22" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G22" s="1"/>
+      <c r="G22" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1">
         <v>1</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>84</v>
@@ -1214,22 +1228,18 @@
       <c r="F23" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="C24" s="1">
-        <v>3</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>88</v>
@@ -1238,7 +1248,30 @@
         <v>89</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>53</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="1">
+        <v>3</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>